<commit_message>
Added auto-py-to-exe modified files
</commit_message>
<xml_diff>
--- a/pyFrame/ScenarioSheet.xlsx
+++ b/pyFrame/ScenarioSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9276"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9276"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioSheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Child Siid</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Norwegian Cruise</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome, Firefox, Ie</t>
+  </si>
+  <si>
+    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -747,12 +756,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -767,12 +782,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -1130,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G13" sqref="G13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1259,10 +1268,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="32"/>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="52"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="39" t="s">
         <v>6</v>
       </c>
@@ -1286,10 +1295,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="38"/>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="53"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="41" t="s">
         <v>7</v>
       </c>
@@ -1311,10 +1320,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="38"/>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="53"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="41" t="s">
         <v>17</v>
       </c>
@@ -1336,11 +1345,11 @@
         <v>3</v>
       </c>
       <c r="D10" s="38"/>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="53"/>
-      <c r="G10" s="49">
+      <c r="F10" s="44"/>
+      <c r="G10" s="51">
         <v>45140</v>
       </c>
       <c r="H10" s="42"/>
@@ -1361,10 +1370,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="38"/>
-      <c r="E11" s="53">
+      <c r="E11" s="44">
         <v>130386</v>
       </c>
-      <c r="F11" s="53"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="41">
         <v>130386</v>
       </c>
@@ -1380,14 +1389,14 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="45" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="53">
+      <c r="E12" s="44">
         <v>130386</v>
       </c>
-      <c r="F12" s="53"/>
+      <c r="F12" s="44"/>
       <c r="G12" s="20">
         <v>130386</v>
       </c>
@@ -1403,16 +1412,16 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="46" t="s">
-        <v>22</v>
+      <c r="C13" s="45" t="s">
+        <v>24</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="48"/>
+      <c r="E13" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="50"/>
       <c r="G13" s="20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="4"/>
@@ -1423,64 +1432,70 @@
       <c r="N13" s="10"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="51"/>
+      <c r="C14" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="50"/>
+      <c r="G14" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="21"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="57"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
       <c r="N14" s="10"/>
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="3"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="14"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="48"/>
+      <c r="G15" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="53"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="10"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="14"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="15"/>
@@ -1497,22 +1512,39 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="1"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:15" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="1"/>
       <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" s="1"/>
+      <c r="I20" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <protectedRanges>
-    <protectedRange password="EFB8" sqref="G8:H14 L8:M14" name="Range1"/>
+    <protectedRange password="EFB8" sqref="G8:H15 L8:M15" name="Range1"/>
   </protectedRanges>
-  <mergeCells count="42">
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
+  <mergeCells count="47">
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
     <mergeCell ref="J3:M6"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -1527,20 +1559,25 @@
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="C3:H6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="J7:K7"/>
@@ -1548,11 +1585,11 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="L8:M8">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="fail">

</xml_diff>